<commit_message>
Testes Mapas returnTo2b Recristalizacao
</commit_message>
<xml_diff>
--- a/Trabalho 2/Meta 2/ResultadosJP.xlsx
+++ b/Trabalho 2/Meta 2/ResultadosJP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Documents\GitHub\Projeto-IAA\Trabalho 2\Meta 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22BB6DC-29CC-445C-8612-827210053E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67666AF-8F39-4AFF-BF8C-CD0AC19703F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{1C22F075-1BF0-EA43-8A90-9BDC22ECA8ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{1C22F075-1BF0-EA43-8A90-9BDC22ECA8ED}"/>
   </bookViews>
   <sheets>
     <sheet name="NoObstacles" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="431">
   <si>
     <t>Trepa Colinas</t>
   </si>
@@ -1134,6 +1134,201 @@
   </si>
   <si>
     <t>2384258p.m._HillClimberOptimiser.csv</t>
+  </si>
+  <si>
+    <t>Funcao de Escalonamento</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>Temp na melhor solução</t>
+  </si>
+  <si>
+    <t>Adaptative Simulated Annealing</t>
+  </si>
+  <si>
+    <t>1 9 8 7 5 6 3 4 2</t>
+  </si>
+  <si>
+    <t>24104535p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>1 4 9 8 7 5 6 3 2</t>
+  </si>
+  <si>
+    <t>24104748p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>1 2 4 9 8 7 6 5 3</t>
+  </si>
+  <si>
+    <t>24110007p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>1 5 7 8 9 4 2 3 6</t>
+  </si>
+  <si>
+    <t>24110134p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>1 4 7 8 9 2 3 6 5</t>
+  </si>
+  <si>
+    <t>24110323p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24110539p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24110626p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24110712p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24110827p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24110852p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24111023p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24111119p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24111204p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24111221p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24111330p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24111410p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24111638p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24111847p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24112204p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24112510p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>14 4 13 5 7 12 17 2 1 15 10 3 6 9 16 11 8</t>
+  </si>
+  <si>
+    <t>24113217p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>1 17 15 4 5 7 10 2 14 16 13 8 11 9 12 3 6</t>
+  </si>
+  <si>
+    <t>24113445p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>15 17 14 10 16 13 7 8 11 12 9 4 5 6 3 2 1</t>
+  </si>
+  <si>
+    <t>24113557p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>16 8 11 12 9 14 3 6 7 17 15 2 4 5 13 10 1</t>
+  </si>
+  <si>
+    <t>24114145p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>15 2 11 8 7 16 9 12 6 5 13 3 1 10 4 14 17</t>
+  </si>
+  <si>
+    <t>24114355p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>1 10 3 6 7 5 13 14 17 15 2 4 16 12 9 11 8</t>
+  </si>
+  <si>
+    <t>24114456p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>1 15 17 13 5 3 10 2 14 4 16 12 9 11 8 7 6</t>
+  </si>
+  <si>
+    <t>24114804p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>15 17 2 14 4 13 7 8 11 9 12 16 5 6 3 10 1</t>
+  </si>
+  <si>
+    <t>24115140p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>3 16 12 9 11 8 7 6 5 13 4 14 2 17 15 1 10</t>
+  </si>
+  <si>
+    <t>24115314p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>3 5 11 8 7 6 9 12 16 13 4 14 2 17 15 1 10</t>
+  </si>
+  <si>
+    <t>24115422p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>24115913p.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>25120116a.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>25120303a.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>25120441a.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>3 6 5 7 8 11 12 9 16 13 4 14 2 17 15 1 10</t>
+  </si>
+  <si>
+    <t>25120601a.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>1 10 13 5 3 6 7 8 11 12 9 16 4 14 2 17 15</t>
+  </si>
+  <si>
+    <t>25122324a.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>3 6 7 5 13 14 2 4 12 9 8 11 16 10 1 15 17</t>
+  </si>
+  <si>
+    <t>25122658a.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>3 10 1 15 17 2 14 4 13 16 9 12 11 8 7 6 5</t>
+  </si>
+  <si>
+    <t>25122909a.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>3 10 1 15 17 2 14 4 16 9 12 11 8 7 6 5 13</t>
+  </si>
+  <si>
+    <t>25123259a.m._SimulatedAnnealingOptimiser.csv</t>
+  </si>
+  <si>
+    <t>3 5 13 4 10 1 15 17 2 14 16 9 12 6 7 8 11</t>
+  </si>
+  <si>
+    <t>25123437a.m._SimulatedAnnealingOptimiser.csv</t>
   </si>
 </sst>
 </file>
@@ -1183,9 +1378,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3448,15 +3644,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35482D3B-BB67-AC4D-83E5-7AF77605C8BE}">
-  <dimension ref="A1:N89"/>
+  <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80:H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="19.69921875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="15.59765625" customWidth="1"/>
+    <col min="6" max="6" width="18.296875" customWidth="1"/>
+    <col min="7" max="7" width="27.69921875" customWidth="1"/>
+    <col min="8" max="8" width="15.8984375" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="19.3984375" customWidth="1"/>
+    <col min="11" max="11" width="21.3984375" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="14" max="14" width="12.59765625" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
@@ -4786,7 +4993,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>180</v>
       </c>
@@ -4812,7 +5019,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>181</v>
       </c>
@@ -4841,7 +5048,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>183</v>
       </c>
@@ -4867,18 +5074,18 @@
         <v>365</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:16" ht="21" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D77" t="s">
         <v>6</v>
       </c>
-      <c r="H77" t="s">
+      <c r="J77" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
         <v>5</v>
       </c>
@@ -4888,73 +5095,792 @@
       <c r="F78" t="s">
         <v>129</v>
       </c>
+      <c r="G78" t="s">
+        <v>366</v>
+      </c>
       <c r="H78" t="s">
+        <v>367</v>
+      </c>
+      <c r="J78" t="s">
         <v>10</v>
       </c>
-      <c r="I78" t="s">
+      <c r="K78" t="s">
+        <v>368</v>
+      </c>
+      <c r="L78" t="s">
         <v>8</v>
       </c>
-      <c r="J78" t="s">
+      <c r="M78" t="s">
         <v>9</v>
       </c>
-      <c r="K78" t="s">
+      <c r="N78" t="s">
         <v>11</v>
       </c>
-      <c r="L78" t="s">
+      <c r="O78" t="s">
         <v>12</v>
       </c>
-      <c r="M78" t="s">
+      <c r="P78" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>100</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>100000</v>
+      </c>
+      <c r="G80" t="s">
+        <v>369</v>
+      </c>
+      <c r="H80">
+        <v>0.5</v>
+      </c>
+      <c r="J80">
+        <v>100</v>
+      </c>
+      <c r="K80">
+        <v>0.19073490000000001</v>
+      </c>
+      <c r="L80" t="s">
+        <v>370</v>
+      </c>
+      <c r="M80">
+        <v>46</v>
+      </c>
+      <c r="N80">
+        <v>73</v>
+      </c>
+      <c r="O80" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>100</v>
+      </c>
+      <c r="E81">
+        <v>500</v>
+      </c>
+      <c r="F81">
+        <v>100000</v>
+      </c>
+      <c r="G81" t="s">
+        <v>369</v>
+      </c>
+      <c r="H81">
+        <v>0.5</v>
+      </c>
+      <c r="J81">
+        <v>100</v>
+      </c>
+      <c r="K81">
+        <v>4.7683719999999999E-2</v>
+      </c>
+      <c r="L81" t="s">
+        <v>372</v>
+      </c>
+      <c r="M81">
+        <v>69</v>
+      </c>
+      <c r="N81">
+        <v>69</v>
+      </c>
+      <c r="O81" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>100</v>
+      </c>
+      <c r="E82">
+        <v>1000</v>
+      </c>
+      <c r="F82">
+        <v>100000</v>
+      </c>
+      <c r="G82" t="s">
+        <v>369</v>
+      </c>
+      <c r="H82">
+        <v>0.5</v>
+      </c>
+      <c r="J82">
+        <v>100</v>
+      </c>
+      <c r="K82">
+        <v>5.9604640000000004E-3</v>
+      </c>
+      <c r="L82" t="s">
+        <v>374</v>
+      </c>
+      <c r="M82">
+        <v>60</v>
+      </c>
+      <c r="N82">
+        <v>65</v>
+      </c>
+      <c r="O82" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>100</v>
+      </c>
+      <c r="E83">
+        <v>1500</v>
+      </c>
+      <c r="F83">
+        <v>100000</v>
+      </c>
+      <c r="G83" t="s">
+        <v>369</v>
+      </c>
+      <c r="H83">
+        <v>0.5</v>
+      </c>
+      <c r="J83">
+        <v>100</v>
+      </c>
+      <c r="K83">
+        <v>2.3841859999999999E-2</v>
+      </c>
+      <c r="L83" t="s">
+        <v>376</v>
+      </c>
+      <c r="M83">
+        <v>27</v>
+      </c>
+      <c r="N83">
+        <v>75</v>
+      </c>
+      <c r="O83" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>100</v>
+      </c>
+      <c r="E84">
+        <v>2000</v>
+      </c>
+      <c r="F84">
+        <v>100000</v>
+      </c>
+      <c r="G84" t="s">
+        <v>369</v>
+      </c>
+      <c r="H84">
+        <v>0.5</v>
+      </c>
+      <c r="J84">
+        <v>100</v>
+      </c>
+      <c r="K84" s="2">
+        <v>7.2759580000000004E-7</v>
+      </c>
+      <c r="L84" t="s">
+        <v>378</v>
+      </c>
+      <c r="M84">
+        <v>95</v>
+      </c>
+      <c r="N84">
+        <v>81</v>
+      </c>
+      <c r="O84" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>500</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>100000</v>
+      </c>
+      <c r="G85" t="s">
+        <v>369</v>
+      </c>
+      <c r="H85">
+        <v>0.5</v>
+      </c>
+      <c r="J85">
+        <v>500</v>
+      </c>
+      <c r="K85">
+        <v>0.19073490000000001</v>
+      </c>
+      <c r="L85" t="s">
+        <v>370</v>
+      </c>
+      <c r="M85">
+        <v>46</v>
+      </c>
+      <c r="N85">
+        <v>73</v>
+      </c>
+      <c r="O85" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>500</v>
+      </c>
+      <c r="E86">
+        <v>500</v>
+      </c>
+      <c r="F86">
+        <v>100000</v>
+      </c>
+      <c r="G86" t="s">
+        <v>369</v>
+      </c>
+      <c r="H86">
+        <v>0.5</v>
+      </c>
+      <c r="J86">
+        <v>500</v>
+      </c>
+      <c r="K86">
+        <v>4.7683719999999999E-2</v>
+      </c>
+      <c r="L86" t="s">
+        <v>372</v>
+      </c>
+      <c r="M86">
+        <v>69</v>
+      </c>
+      <c r="N86">
+        <v>69</v>
+      </c>
+      <c r="O86" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>500</v>
+      </c>
+      <c r="E87">
+        <v>1000</v>
+      </c>
+      <c r="F87">
+        <v>100000</v>
+      </c>
+      <c r="G87" t="s">
+        <v>369</v>
+      </c>
+      <c r="H87">
+        <v>0.5</v>
+      </c>
+      <c r="J87">
+        <v>500</v>
+      </c>
+      <c r="K87">
+        <v>2.9802320000000002E-3</v>
+      </c>
+      <c r="L87" t="s">
+        <v>187</v>
+      </c>
+      <c r="M87">
+        <v>115</v>
+      </c>
+      <c r="N87">
+        <v>63</v>
+      </c>
+      <c r="O87" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>500</v>
+      </c>
+      <c r="E88">
+        <v>1500</v>
+      </c>
+      <c r="F88">
+        <v>100000</v>
+      </c>
+      <c r="G88" t="s">
+        <v>369</v>
+      </c>
+      <c r="H88">
+        <v>0.5</v>
+      </c>
+      <c r="J88">
+        <v>500</v>
+      </c>
+      <c r="K88">
+        <v>2.3841859999999999E-2</v>
+      </c>
+      <c r="L88" t="s">
+        <v>376</v>
+      </c>
+      <c r="M88">
+        <v>27</v>
+      </c>
+      <c r="N88">
+        <v>75</v>
+      </c>
+      <c r="O88" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>23</v>
+      </c>
+      <c r="D89">
+        <v>500</v>
+      </c>
+      <c r="E89">
+        <v>2000</v>
+      </c>
+      <c r="F89">
+        <v>100000</v>
+      </c>
+      <c r="G89" t="s">
+        <v>369</v>
+      </c>
+      <c r="H89">
+        <v>0.5</v>
+      </c>
+      <c r="J89">
+        <v>500</v>
+      </c>
+      <c r="K89" s="2">
+        <v>3.5527139999999999E-10</v>
+      </c>
+      <c r="L89" t="s">
+        <v>372</v>
+      </c>
+      <c r="M89">
+        <v>212</v>
+      </c>
+      <c r="N89">
+        <v>69</v>
+      </c>
+      <c r="O89" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>120</v>
+      </c>
+      <c r="D90">
+        <v>1000</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>100000</v>
+      </c>
+      <c r="G90" t="s">
+        <v>369</v>
+      </c>
+      <c r="H90">
+        <v>0.5</v>
+      </c>
+      <c r="J90">
+        <v>10000</v>
+      </c>
+      <c r="K90">
+        <v>0.19073490000000001</v>
+      </c>
+      <c r="L90" t="s">
+        <v>370</v>
+      </c>
+      <c r="M90">
+        <v>46</v>
+      </c>
+      <c r="N90">
+        <v>73</v>
+      </c>
+      <c r="O90" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>122</v>
+      </c>
+      <c r="D91">
+        <v>1000</v>
+      </c>
+      <c r="E91">
+        <v>500</v>
+      </c>
+      <c r="F91">
+        <v>100000</v>
+      </c>
+      <c r="G91" t="s">
+        <v>369</v>
+      </c>
+      <c r="H91">
+        <v>0.5</v>
+      </c>
+      <c r="J91">
+        <v>10000</v>
+      </c>
+      <c r="K91">
+        <v>4.7683719999999999E-2</v>
+      </c>
+      <c r="L91" t="s">
+        <v>372</v>
+      </c>
+      <c r="M91">
+        <v>69</v>
+      </c>
+      <c r="N91">
+        <v>69</v>
+      </c>
+      <c r="O91" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>126</v>
+      </c>
+      <c r="D92">
+        <v>1000</v>
+      </c>
+      <c r="E92">
+        <v>1000</v>
+      </c>
+      <c r="F92">
+        <v>100000</v>
+      </c>
+      <c r="G92" t="s">
+        <v>369</v>
+      </c>
+      <c r="H92">
+        <v>0.5</v>
+      </c>
+      <c r="J92">
+        <v>10000</v>
+      </c>
+      <c r="K92">
+        <v>2.9802320000000002E-3</v>
+      </c>
+      <c r="L92" t="s">
+        <v>187</v>
+      </c>
+      <c r="M92">
+        <v>115</v>
+      </c>
+      <c r="N92">
+        <v>63</v>
+      </c>
+      <c r="O92" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>127</v>
+      </c>
+      <c r="D93">
+        <v>1000</v>
+      </c>
+      <c r="E93">
+        <v>1500</v>
+      </c>
+      <c r="F93">
+        <v>100000</v>
+      </c>
+      <c r="G93" t="s">
+        <v>369</v>
+      </c>
+      <c r="H93">
+        <v>0.5</v>
+      </c>
+      <c r="J93">
+        <v>10000</v>
+      </c>
+      <c r="K93">
+        <v>2.3841859999999999E-2</v>
+      </c>
+      <c r="L93" t="s">
+        <v>376</v>
+      </c>
+      <c r="M93">
+        <v>27</v>
+      </c>
+      <c r="N93">
+        <v>75</v>
+      </c>
+      <c r="O93" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>176</v>
+      </c>
+      <c r="D94">
+        <v>1000</v>
+      </c>
+      <c r="E94">
+        <v>2000</v>
+      </c>
+      <c r="F94">
+        <v>100000</v>
+      </c>
+      <c r="G94" t="s">
+        <v>369</v>
+      </c>
+      <c r="H94">
+        <v>0.5</v>
+      </c>
+      <c r="J94">
+        <v>10000</v>
+      </c>
+      <c r="K94" s="2">
+        <v>3.5527139999999999E-10</v>
+      </c>
+      <c r="L94" t="s">
+        <v>372</v>
+      </c>
+      <c r="M94">
+        <v>212</v>
+      </c>
+      <c r="N94">
+        <v>69</v>
+      </c>
+      <c r="O94" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>177</v>
+      </c>
+      <c r="D95">
+        <v>5000</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>100000</v>
+      </c>
+      <c r="G95" t="s">
+        <v>369</v>
+      </c>
+      <c r="H95">
+        <v>0.5</v>
+      </c>
+      <c r="J95">
+        <v>5000</v>
+      </c>
+      <c r="K95">
+        <v>4.7683719999999999E-2</v>
+      </c>
+      <c r="L95" t="s">
+        <v>370</v>
+      </c>
+      <c r="M95">
+        <v>3634</v>
+      </c>
+      <c r="N95">
+        <v>73</v>
+      </c>
+      <c r="O95" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>178</v>
+      </c>
+      <c r="D96">
+        <v>5000</v>
+      </c>
+      <c r="E96">
+        <v>500</v>
+      </c>
+      <c r="F96">
+        <v>100000</v>
+      </c>
+      <c r="G96" t="s">
+        <v>369</v>
+      </c>
+      <c r="H96">
+        <v>0.5</v>
+      </c>
+      <c r="J96">
+        <v>5000</v>
+      </c>
+      <c r="K96">
+        <v>4.7683719999999999E-2</v>
+      </c>
+      <c r="L96" t="s">
+        <v>372</v>
+      </c>
+      <c r="M96">
+        <v>69</v>
+      </c>
+      <c r="N96">
+        <v>69</v>
+      </c>
+      <c r="O96" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>179</v>
+      </c>
+      <c r="D97">
+        <v>5000</v>
+      </c>
+      <c r="E97">
+        <v>1000</v>
+      </c>
+      <c r="F97">
+        <v>100000</v>
+      </c>
+      <c r="G97" t="s">
+        <v>369</v>
+      </c>
+      <c r="H97">
+        <v>0.5</v>
+      </c>
+      <c r="J97">
+        <v>5000</v>
+      </c>
+      <c r="K97">
+        <v>2.9802320000000002E-3</v>
+      </c>
+      <c r="L97" t="s">
+        <v>187</v>
+      </c>
+      <c r="M97">
+        <v>115</v>
+      </c>
+      <c r="N97">
+        <v>63</v>
+      </c>
+      <c r="O97" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>180</v>
+      </c>
+      <c r="D98">
+        <v>5000</v>
+      </c>
+      <c r="E98">
+        <v>1500</v>
+      </c>
+      <c r="F98">
+        <v>100000</v>
+      </c>
+      <c r="G98" t="s">
+        <v>369</v>
+      </c>
+      <c r="H98">
+        <v>0.5</v>
+      </c>
+      <c r="J98">
+        <v>5000</v>
+      </c>
+      <c r="K98">
+        <v>2.3841859999999999E-2</v>
+      </c>
+      <c r="L98" t="s">
+        <v>376</v>
+      </c>
+      <c r="M98">
+        <v>27</v>
+      </c>
+      <c r="N98">
+        <v>75</v>
+      </c>
+      <c r="O98" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>181</v>
+      </c>
+      <c r="D99">
+        <v>5000</v>
+      </c>
+      <c r="E99">
+        <v>2000</v>
+      </c>
+      <c r="F99">
+        <v>100000</v>
+      </c>
+      <c r="G99" t="s">
+        <v>369</v>
+      </c>
+      <c r="H99">
+        <v>0.5</v>
+      </c>
+      <c r="J99">
+        <v>5000</v>
+      </c>
+      <c r="K99" s="2">
+        <v>3.5527139999999999E-10</v>
+      </c>
+      <c r="L99" t="s">
+        <v>372</v>
+      </c>
+      <c r="M99">
+        <v>212</v>
+      </c>
+      <c r="N99">
+        <v>69</v>
+      </c>
+      <c r="O99" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -4965,21 +5891,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C91D61-F5E8-A647-82E8-F0EDF9A7AD79}">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N91" sqref="N91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="17.5" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="15.09765625" customWidth="1"/>
+    <col min="6" max="6" width="18.59765625" customWidth="1"/>
+    <col min="7" max="7" width="28.8984375" customWidth="1"/>
     <col min="8" max="8" width="35.09765625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="12.3984375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="33.09765625" customWidth="1"/>
+    <col min="12" max="12" width="33.59765625" customWidth="1"/>
+    <col min="13" max="13" width="19.59765625" customWidth="1"/>
+    <col min="14" max="14" width="13.69921875" customWidth="1"/>
+    <col min="15" max="15" width="33.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
@@ -6509,7 +7440,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>190</v>
       </c>
@@ -6535,7 +7466,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>191</v>
       </c>
@@ -6561,7 +7492,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>192</v>
       </c>
@@ -6587,7 +7518,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>229</v>
       </c>
@@ -6613,7 +7544,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>230</v>
       </c>
@@ -6639,7 +7570,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>231</v>
       </c>
@@ -6665,18 +7596,18 @@
         <v>362</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:16" ht="21" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D74" t="s">
         <v>6</v>
       </c>
-      <c r="H74" t="s">
+      <c r="J74" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
         <v>5</v>
       </c>
@@ -6686,73 +7617,792 @@
       <c r="F75" t="s">
         <v>129</v>
       </c>
+      <c r="G75" t="s">
+        <v>366</v>
+      </c>
       <c r="H75" t="s">
+        <v>367</v>
+      </c>
+      <c r="J75" t="s">
         <v>10</v>
       </c>
-      <c r="I75" t="s">
+      <c r="K75" t="s">
+        <v>368</v>
+      </c>
+      <c r="L75" t="s">
         <v>8</v>
       </c>
-      <c r="J75" t="s">
+      <c r="M75" t="s">
         <v>9</v>
       </c>
-      <c r="K75" t="s">
+      <c r="N75" t="s">
         <v>11</v>
       </c>
-      <c r="L75" t="s">
+      <c r="O75" t="s">
         <v>12</v>
       </c>
-      <c r="M75" t="s">
+      <c r="P75" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>100</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>100000</v>
+      </c>
+      <c r="G77" t="s">
+        <v>369</v>
+      </c>
+      <c r="H77">
+        <v>0.5</v>
+      </c>
+      <c r="J77">
+        <v>100</v>
+      </c>
+      <c r="K77">
+        <v>7.4505809999999997E-4</v>
+      </c>
+      <c r="L77" t="s">
+        <v>395</v>
+      </c>
+      <c r="M77">
+        <v>67</v>
+      </c>
+      <c r="N77">
+        <v>137</v>
+      </c>
+      <c r="O77" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>100</v>
+      </c>
+      <c r="E78">
+        <v>500</v>
+      </c>
+      <c r="F78">
+        <v>100000</v>
+      </c>
+      <c r="G78" t="s">
+        <v>369</v>
+      </c>
+      <c r="H78">
+        <v>0.5</v>
+      </c>
+      <c r="J78">
+        <v>100</v>
+      </c>
+      <c r="K78" s="2">
+        <v>4.6566130000000003E-5</v>
+      </c>
+      <c r="L78" t="s">
+        <v>397</v>
+      </c>
+      <c r="M78">
+        <v>97</v>
+      </c>
+      <c r="N78">
+        <v>129</v>
+      </c>
+      <c r="O78" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>100</v>
+      </c>
+      <c r="E79">
+        <v>1000</v>
+      </c>
+      <c r="F79">
+        <v>100000</v>
+      </c>
+      <c r="G79" t="s">
+        <v>369</v>
+      </c>
+      <c r="H79">
+        <v>0.5</v>
+      </c>
+      <c r="J79">
+        <v>100</v>
+      </c>
+      <c r="K79" s="2">
+        <v>2.3283060000000001E-5</v>
+      </c>
+      <c r="L79" t="s">
+        <v>399</v>
+      </c>
+      <c r="M79">
+        <v>90</v>
+      </c>
+      <c r="N79">
+        <v>120</v>
+      </c>
+      <c r="O79" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>100</v>
+      </c>
+      <c r="E80">
+        <v>1500</v>
+      </c>
+      <c r="F80">
+        <v>100000</v>
+      </c>
+      <c r="G80" t="s">
+        <v>369</v>
+      </c>
+      <c r="H80">
+        <v>0.5</v>
+      </c>
+      <c r="J80">
+        <v>100</v>
+      </c>
+      <c r="K80" s="2">
+        <v>1.8189889999999999E-7</v>
+      </c>
+      <c r="L80" t="s">
+        <v>401</v>
+      </c>
+      <c r="M80">
+        <v>86</v>
+      </c>
+      <c r="N80">
+        <v>140</v>
+      </c>
+      <c r="O80" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>100</v>
+      </c>
+      <c r="E81">
+        <v>2000</v>
+      </c>
+      <c r="F81">
+        <v>100000</v>
+      </c>
+      <c r="G81" t="s">
+        <v>369</v>
+      </c>
+      <c r="H81">
+        <v>0.5</v>
+      </c>
+      <c r="J81">
+        <v>100</v>
+      </c>
+      <c r="K81">
+        <v>3.7252900000000002E-4</v>
+      </c>
+      <c r="L81" t="s">
+        <v>403</v>
+      </c>
+      <c r="M81">
+        <v>84</v>
+      </c>
+      <c r="N81">
+        <v>127</v>
+      </c>
+      <c r="O81" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>1000</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>100000</v>
+      </c>
+      <c r="G82" t="s">
+        <v>369</v>
+      </c>
+      <c r="H82">
+        <v>0.5</v>
+      </c>
+      <c r="J82">
+        <v>1000</v>
+      </c>
+      <c r="K82" s="2">
+        <v>1.421085E-9</v>
+      </c>
+      <c r="L82" t="s">
+        <v>405</v>
+      </c>
+      <c r="M82">
+        <v>297</v>
+      </c>
+      <c r="N82">
+        <v>89</v>
+      </c>
+      <c r="O82" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>1000</v>
+      </c>
+      <c r="E83">
+        <v>500</v>
+      </c>
+      <c r="F83">
+        <v>100000</v>
+      </c>
+      <c r="G83" t="s">
+        <v>369</v>
+      </c>
+      <c r="H83">
+        <v>0.5</v>
+      </c>
+      <c r="J83">
+        <v>1000</v>
+      </c>
+      <c r="K83" s="2">
+        <v>1.110223E-11</v>
+      </c>
+      <c r="L83" t="s">
+        <v>407</v>
+      </c>
+      <c r="M83">
+        <v>477</v>
+      </c>
+      <c r="N83">
+        <v>95</v>
+      </c>
+      <c r="O83" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>1000</v>
+      </c>
+      <c r="E84">
+        <v>1000</v>
+      </c>
+      <c r="F84">
+        <v>100000</v>
+      </c>
+      <c r="G84" t="s">
+        <v>369</v>
+      </c>
+      <c r="H84">
+        <v>0.5</v>
+      </c>
+      <c r="J84">
+        <v>1000</v>
+      </c>
+      <c r="K84" s="2">
+        <v>2.2737369999999999E-8</v>
+      </c>
+      <c r="L84" t="s">
+        <v>409</v>
+      </c>
+      <c r="M84">
+        <v>387</v>
+      </c>
+      <c r="N84">
+        <v>92</v>
+      </c>
+      <c r="O84" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>1000</v>
+      </c>
+      <c r="E85">
+        <v>1500</v>
+      </c>
+      <c r="F85">
+        <v>100000</v>
+      </c>
+      <c r="G85" t="s">
+        <v>369</v>
+      </c>
+      <c r="H85">
+        <v>0.5</v>
+      </c>
+      <c r="J85">
+        <v>1000</v>
+      </c>
+      <c r="K85" s="2">
+        <v>8.470329E-17</v>
+      </c>
+      <c r="L85" t="s">
+        <v>411</v>
+      </c>
+      <c r="M85">
+        <v>969</v>
+      </c>
+      <c r="N85">
+        <v>85</v>
+      </c>
+      <c r="O85" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>23</v>
+      </c>
+      <c r="D86">
+        <v>1000</v>
+      </c>
+      <c r="E86">
+        <v>2000</v>
+      </c>
+      <c r="F86">
+        <v>100000</v>
+      </c>
+      <c r="G86" t="s">
+        <v>369</v>
+      </c>
+      <c r="H86">
+        <v>0.5</v>
+      </c>
+      <c r="J86">
+        <v>1000</v>
+      </c>
+      <c r="K86" s="2">
+        <v>4.3368089999999999E-14</v>
+      </c>
+      <c r="L86" t="s">
+        <v>413</v>
+      </c>
+      <c r="M86">
+        <v>820</v>
+      </c>
+      <c r="N86">
+        <v>91</v>
+      </c>
+      <c r="O86" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>120</v>
+      </c>
+      <c r="D87">
+        <v>5000</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>100000</v>
+      </c>
+      <c r="G87" t="s">
+        <v>369</v>
+      </c>
+      <c r="H87">
+        <v>0.5</v>
+      </c>
+      <c r="J87">
+        <v>5000</v>
+      </c>
+      <c r="K87" s="2">
+        <v>1.421085E-9</v>
+      </c>
+      <c r="L87" t="s">
+        <v>405</v>
+      </c>
+      <c r="M87">
+        <v>297</v>
+      </c>
+      <c r="N87">
+        <v>89</v>
+      </c>
+      <c r="O87" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>122</v>
+      </c>
+      <c r="D88">
+        <v>5000</v>
+      </c>
+      <c r="E88">
+        <v>500</v>
+      </c>
+      <c r="F88">
+        <v>100000</v>
+      </c>
+      <c r="G88" t="s">
+        <v>369</v>
+      </c>
+      <c r="H88">
+        <v>0.5</v>
+      </c>
+      <c r="J88">
+        <v>5000</v>
+      </c>
+      <c r="K88" s="2">
+        <v>1.110223E-11</v>
+      </c>
+      <c r="L88" t="s">
+        <v>407</v>
+      </c>
+      <c r="M88">
+        <v>477</v>
+      </c>
+      <c r="N88">
+        <v>95</v>
+      </c>
+      <c r="O88" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>126</v>
+      </c>
+      <c r="D89">
+        <v>5000</v>
+      </c>
+      <c r="E89">
+        <v>1000</v>
+      </c>
+      <c r="F89">
+        <v>100000</v>
+      </c>
+      <c r="G89" t="s">
+        <v>369</v>
+      </c>
+      <c r="H89">
+        <v>0.5</v>
+      </c>
+      <c r="J89">
+        <v>5000</v>
+      </c>
+      <c r="K89" s="2">
+        <v>2.2737369999999999E-8</v>
+      </c>
+      <c r="L89" t="s">
+        <v>409</v>
+      </c>
+      <c r="M89">
+        <v>387</v>
+      </c>
+      <c r="N89">
+        <v>92</v>
+      </c>
+      <c r="O89" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>127</v>
+      </c>
+      <c r="D90">
+        <v>5000</v>
+      </c>
+      <c r="E90">
+        <v>1500</v>
+      </c>
+      <c r="F90">
+        <v>100000</v>
+      </c>
+      <c r="G90" t="s">
+        <v>369</v>
+      </c>
+      <c r="H90">
+        <v>0.5</v>
+      </c>
+      <c r="J90">
+        <v>5000</v>
+      </c>
+      <c r="K90" s="2">
+        <v>8.470329E-17</v>
+      </c>
+      <c r="L90" t="s">
+        <v>411</v>
+      </c>
+      <c r="M90">
+        <v>969</v>
+      </c>
+      <c r="N90">
+        <v>85</v>
+      </c>
+      <c r="O90" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>176</v>
+      </c>
+      <c r="D91">
+        <v>5000</v>
+      </c>
+      <c r="E91">
+        <v>2000</v>
+      </c>
+      <c r="F91">
+        <v>100000</v>
+      </c>
+      <c r="G91" t="s">
+        <v>369</v>
+      </c>
+      <c r="H91">
+        <v>0.5</v>
+      </c>
+      <c r="J91">
+        <v>5000</v>
+      </c>
+      <c r="K91" s="2">
+        <v>4.2351649999999999E-17</v>
+      </c>
+      <c r="L91" t="s">
+        <v>419</v>
+      </c>
+      <c r="M91">
+        <v>1093</v>
+      </c>
+      <c r="N91">
+        <v>77</v>
+      </c>
+      <c r="O91" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>177</v>
+      </c>
+      <c r="D92">
+        <v>5000</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>100000</v>
+      </c>
+      <c r="G92" t="s">
+        <v>369</v>
+      </c>
+      <c r="H92">
+        <v>0.98</v>
+      </c>
+      <c r="J92">
+        <v>5000</v>
+      </c>
+      <c r="K92">
+        <v>1.2456069999999999</v>
+      </c>
+      <c r="L92" t="s">
+        <v>421</v>
+      </c>
+      <c r="M92">
+        <v>1697</v>
+      </c>
+      <c r="N92">
+        <v>85</v>
+      </c>
+      <c r="O92" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>178</v>
+      </c>
+      <c r="D93">
+        <v>5000</v>
+      </c>
+      <c r="E93">
+        <v>500</v>
+      </c>
+      <c r="F93">
+        <v>100000</v>
+      </c>
+      <c r="G93" t="s">
+        <v>369</v>
+      </c>
+      <c r="H93">
+        <v>0.98</v>
+      </c>
+      <c r="J93">
+        <v>5000</v>
+      </c>
+      <c r="K93">
+        <v>0.83157769999999998</v>
+      </c>
+      <c r="L93" t="s">
+        <v>423</v>
+      </c>
+      <c r="M93">
+        <v>1384</v>
+      </c>
+      <c r="N93">
+        <v>99</v>
+      </c>
+      <c r="O93" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>179</v>
+      </c>
+      <c r="D94">
+        <v>5000</v>
+      </c>
+      <c r="E94">
+        <v>1000</v>
+      </c>
+      <c r="F94">
+        <v>100000</v>
+      </c>
+      <c r="G94" t="s">
+        <v>369</v>
+      </c>
+      <c r="H94">
+        <v>0.98</v>
+      </c>
+      <c r="J94">
+        <v>5000</v>
+      </c>
+      <c r="K94">
+        <v>1.059717</v>
+      </c>
+      <c r="L94" t="s">
+        <v>425</v>
+      </c>
+      <c r="M94">
+        <v>1582</v>
+      </c>
+      <c r="N94">
+        <v>79</v>
+      </c>
+      <c r="O94" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>180</v>
+      </c>
+      <c r="D95">
+        <v>5000</v>
+      </c>
+      <c r="E95">
+        <v>1500</v>
+      </c>
+      <c r="F95">
+        <v>100000</v>
+      </c>
+      <c r="G95" t="s">
+        <v>369</v>
+      </c>
+      <c r="H95">
+        <v>0.98</v>
+      </c>
+      <c r="J95">
+        <v>5000</v>
+      </c>
+      <c r="K95">
+        <v>1.017752</v>
+      </c>
+      <c r="L95" t="s">
+        <v>427</v>
+      </c>
+      <c r="M95">
+        <v>2137</v>
+      </c>
+      <c r="N95">
+        <v>81</v>
+      </c>
+      <c r="O95" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>181</v>
+      </c>
+      <c r="D96">
+        <v>5000</v>
+      </c>
+      <c r="E96">
+        <v>2000</v>
+      </c>
+      <c r="F96">
+        <v>100000</v>
+      </c>
+      <c r="G96" t="s">
+        <v>369</v>
+      </c>
+      <c r="H96">
+        <v>0.98</v>
+      </c>
+      <c r="J96">
+        <v>5000</v>
+      </c>
+      <c r="K96">
+        <v>0.6141778</v>
+      </c>
+      <c r="L96" t="s">
+        <v>429</v>
+      </c>
+      <c r="M96">
+        <v>3691</v>
+      </c>
+      <c r="N96">
+        <v>89</v>
+      </c>
+      <c r="O96" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -7225,7 +8875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD78113-BF29-4DE2-BB0B-C375FBE02098}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>